<commit_message>
Added Apple M3 results
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\shared\arm-instruction-time\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Devel/arm-instruction-time/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469CC024-B06A-45F8-A300-C54E226002D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6406F677-0B02-1841-A6BB-163769D744F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8745" yWindow="2220" windowWidth="22575" windowHeight="18735" xr2:uid="{D46DF09C-373D-4B8F-933A-76CBCC1CC5EF}"/>
+    <workbookView xWindow="11040" yWindow="3040" windowWidth="29000" windowHeight="18740" xr2:uid="{D46DF09C-373D-4B8F-933A-76CBCC1CC5EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Ignoring empty loop time" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>Apple M1</t>
   </si>
@@ -183,6 +183,9 @@
   </si>
   <si>
     <t>Neoverse V2</t>
+  </si>
+  <si>
+    <t>Apple M3</t>
   </si>
 </sst>
 </file>
@@ -744,31 +747,33 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AB42"/>
+  <dimension ref="B1:AG42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="1.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="1" customWidth="1"/>
-    <col min="4" max="5" width="1.140625" customWidth="1"/>
-    <col min="6" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="10" width="1.140625" customWidth="1"/>
-    <col min="11" max="13" width="8.7109375" customWidth="1"/>
-    <col min="14" max="15" width="1.140625" customWidth="1"/>
-    <col min="16" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="19" width="1.140625" customWidth="1"/>
-    <col min="20" max="22" width="8.7109375" customWidth="1"/>
-    <col min="23" max="24" width="1.140625" customWidth="1"/>
-    <col min="25" max="27" width="8.7109375" customWidth="1"/>
-    <col min="28" max="28" width="1.140625" customWidth="1"/>
+    <col min="1" max="2" width="1.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" style="1" customWidth="1"/>
+    <col min="4" max="5" width="1.1640625" customWidth="1"/>
+    <col min="6" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="10" width="1.1640625" customWidth="1"/>
+    <col min="11" max="13" width="8.6640625" customWidth="1"/>
+    <col min="14" max="15" width="1.1640625" customWidth="1"/>
+    <col min="16" max="17" width="8.6640625" customWidth="1"/>
+    <col min="18" max="19" width="1.1640625" customWidth="1"/>
+    <col min="20" max="22" width="8.6640625" customWidth="1"/>
+    <col min="23" max="24" width="1.1640625" customWidth="1"/>
+    <col min="25" max="27" width="8.6640625" customWidth="1"/>
+    <col min="28" max="29" width="1.1640625" customWidth="1"/>
+    <col min="30" max="32" width="8.6640625" customWidth="1"/>
+    <col min="33" max="33" width="1.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="3.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:33" ht="4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
         <v>19</v>
@@ -808,8 +813,15 @@
       <c r="Z2" s="22"/>
       <c r="AA2" s="22"/>
       <c r="AB2" s="7"/>
-    </row>
-    <row r="3" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE2" s="22"/>
+      <c r="AF2" s="22"/>
+      <c r="AG2" s="7"/>
+    </row>
+    <row r="3" spans="2:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
       <c r="C3" s="2" t="s">
         <v>21</v>
@@ -848,8 +860,14 @@
       <c r="Z3" s="23"/>
       <c r="AA3" s="23"/>
       <c r="AB3" s="9"/>
-    </row>
-    <row r="4" spans="2:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="AD3" s="23">
+        <v>4</v>
+      </c>
+      <c r="AE3" s="23"/>
+      <c r="AF3" s="23"/>
+      <c r="AG3" s="9"/>
+    </row>
+    <row r="4" spans="2:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="14"/>
       <c r="C4" s="15" t="s">
         <v>35</v>
@@ -907,8 +925,19 @@
         <v>36</v>
       </c>
       <c r="AB4" s="16"/>
-    </row>
-    <row r="5" spans="2:28" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG4" s="16"/>
+    </row>
+    <row r="5" spans="2:33" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="8"/>
       <c r="D5" s="9"/>
       <c r="E5" s="8"/>
@@ -920,8 +949,9 @@
       <c r="S5" s="8"/>
       <c r="W5" s="9"/>
       <c r="AB5" s="9"/>
-    </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AG5" s="9"/>
+    </row>
+    <row r="6" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B6" s="8"/>
       <c r="C6" t="s">
         <v>4</v>
@@ -987,8 +1017,20 @@
         <v>0.53846153846153832</v>
       </c>
       <c r="AB6" s="9"/>
-    </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD6" s="3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="AE6" s="3">
+        <f>1/($AD$3*AD6)</f>
+        <v>7.8125</v>
+      </c>
+      <c r="AF6" s="20">
+        <f>(AD6*$AD$3 - $P6*$P$3)/($P6*$P$3)</f>
+        <v>0.36752136752136749</v>
+      </c>
+      <c r="AG6" s="9"/>
+    </row>
+    <row r="7" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B7" s="8"/>
       <c r="C7" t="s">
         <v>5</v>
@@ -1054,8 +1096,20 @@
         <v>-0.1297591297591297</v>
       </c>
       <c r="AB7" s="9"/>
-    </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD7" s="3">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AE7" s="3">
+        <f t="shared" ref="AE7:AE32" si="8">1/($AD$3*AD7)</f>
+        <v>6.5789473684210531</v>
+      </c>
+      <c r="AF7" s="20">
+        <f t="shared" ref="AF7:AF32" si="9">(AD7*$AD$3 - $P7*$P$3)/($P7*$P$3)</f>
+        <v>-0.40947940947940953</v>
+      </c>
+      <c r="AG7" s="9"/>
+    </row>
+    <row r="8" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B8" s="8"/>
       <c r="C8" t="s">
         <v>6</v>
@@ -1092,7 +1146,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" ref="Q8:Q36" si="8">1/($P$3*P8)</f>
+        <f t="shared" ref="Q8:Q36" si="10">1/($P$3*P8)</f>
         <v>3.8850038850038846</v>
       </c>
       <c r="R8" s="9"/>
@@ -1121,8 +1175,20 @@
         <v>0.34265734265734266</v>
       </c>
       <c r="AB8" s="9"/>
-    </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD8" s="3">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="AE8" s="3">
+        <f t="shared" si="8"/>
+        <v>3.6764705882352939</v>
+      </c>
+      <c r="AF8" s="20">
+        <f t="shared" si="9"/>
+        <v>5.6721056721056727E-2</v>
+      </c>
+      <c r="AG8" s="9"/>
+    </row>
+    <row r="9" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" t="s">
         <v>7</v>
@@ -1159,7 +1225,7 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="Q9" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.935995302407516</v>
       </c>
       <c r="R9" s="9"/>
@@ -1188,8 +1254,20 @@
         <v>5.2847915443335986E-3</v>
       </c>
       <c r="AB9" s="9"/>
-    </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD9" s="3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AE9" s="3">
+        <f t="shared" si="8"/>
+        <v>3.5714285714285712</v>
+      </c>
+      <c r="AF9" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.17792131532589545</v>
+      </c>
+      <c r="AG9" s="9"/>
+    </row>
+    <row r="10" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="C10" t="s">
         <v>8</v>
@@ -1226,7 +1304,7 @@
         <v>0.38800000000000001</v>
       </c>
       <c r="Q10" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99127676447264057</v>
       </c>
       <c r="R10" s="9"/>
@@ -1255,8 +1333,20 @@
         <v>-7.137192704203107E-3</v>
       </c>
       <c r="AB10" s="9"/>
-    </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD10" s="3">
+        <v>0.253</v>
+      </c>
+      <c r="AE10" s="3">
+        <f t="shared" si="8"/>
+        <v>0.98814229249011853</v>
+      </c>
+      <c r="AF10" s="20">
+        <f t="shared" si="9"/>
+        <v>3.1720856463123208E-3</v>
+      </c>
+      <c r="AG10" s="9"/>
+    </row>
+    <row r="11" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B11" s="8"/>
       <c r="C11" t="s">
         <v>9</v>
@@ -1293,7 +1383,7 @@
         <v>0.193</v>
       </c>
       <c r="Q11" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.9928258270227182</v>
       </c>
       <c r="R11" s="9"/>
@@ -1322,8 +1412,20 @@
         <v>-5.1813471502590493E-3</v>
       </c>
       <c r="AB11" s="9"/>
-    </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD11" s="19">
+        <v>0.129</v>
+      </c>
+      <c r="AE11" s="3">
+        <f t="shared" si="8"/>
+        <v>1.9379844961240309</v>
+      </c>
+      <c r="AF11" s="20">
+        <f t="shared" si="9"/>
+        <v>2.829812674372258E-2</v>
+      </c>
+      <c r="AG11" s="9"/>
+    </row>
+    <row r="12" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B12" s="8"/>
       <c r="C12" t="s">
         <v>10</v>
@@ -1360,7 +1462,7 @@
         <v>0.193</v>
       </c>
       <c r="Q12" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.9928258270227182</v>
       </c>
       <c r="R12" s="9"/>
@@ -1389,8 +1491,20 @@
         <v>-5.1813471502590493E-3</v>
       </c>
       <c r="AB12" s="9"/>
-    </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD12" s="19">
+        <v>0.126</v>
+      </c>
+      <c r="AE12" s="3">
+        <f t="shared" si="8"/>
+        <v>1.9841269841269842</v>
+      </c>
+      <c r="AF12" s="20">
+        <f t="shared" si="9"/>
+        <v>4.3842168194499391E-3</v>
+      </c>
+      <c r="AG12" s="9"/>
+    </row>
+    <row r="13" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B13" s="8"/>
       <c r="C13" t="s">
         <v>23</v>
@@ -1427,7 +1541,7 @@
         <v>2.3109999999999999</v>
       </c>
       <c r="Q13" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.16642811969510368</v>
       </c>
       <c r="R13" s="9"/>
@@ -1456,8 +1570,20 @@
         <v>-0.66714376060979264</v>
       </c>
       <c r="AB13" s="9"/>
-    </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD13" s="3">
+        <v>0.496</v>
+      </c>
+      <c r="AE13" s="3">
+        <f t="shared" si="8"/>
+        <v>0.50403225806451613</v>
+      </c>
+      <c r="AF13" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.6698066105249143</v>
+      </c>
+      <c r="AG13" s="9"/>
+    </row>
+    <row r="14" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B14" s="8"/>
       <c r="C14" t="s">
         <v>11</v>
@@ -1494,7 +1620,7 @@
         <v>0.193</v>
       </c>
       <c r="Q14" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.9928258270227182</v>
       </c>
       <c r="R14" s="9"/>
@@ -1523,8 +1649,20 @@
         <v>-5.1813471502590493E-3</v>
       </c>
       <c r="AB14" s="9"/>
-    </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD14" s="3">
+        <v>0.124</v>
+      </c>
+      <c r="AE14" s="3">
+        <f t="shared" si="8"/>
+        <v>2.0161290322580645</v>
+      </c>
+      <c r="AF14" s="20">
+        <f t="shared" si="9"/>
+        <v>-1.155838979673182E-2</v>
+      </c>
+      <c r="AG14" s="9"/>
+    </row>
+    <row r="15" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B15" s="8"/>
       <c r="C15" t="s">
         <v>12</v>
@@ -1561,7 +1699,7 @@
         <v>0.29399999999999998</v>
       </c>
       <c r="Q15" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.3082155939298796</v>
       </c>
       <c r="R15" s="9"/>
@@ -1590,8 +1728,20 @@
         <v>-0.34275248560962834</v>
       </c>
       <c r="AB15" s="9"/>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD15" s="3">
+        <v>0.124</v>
+      </c>
+      <c r="AE15" s="3">
+        <f t="shared" si="8"/>
+        <v>2.0161290322580645</v>
+      </c>
+      <c r="AF15" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.3511250654107797</v>
+      </c>
+      <c r="AG15" s="9"/>
+    </row>
+    <row r="16" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
       <c r="C16" t="s">
         <v>24</v>
@@ -1628,7 +1778,7 @@
         <v>0.105</v>
       </c>
       <c r="Q16" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6630036630036629</v>
       </c>
       <c r="R16" s="9"/>
@@ -1657,8 +1807,20 @@
         <v>0.21904761904761891</v>
       </c>
       <c r="AB16" s="9"/>
-    </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD16" s="3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="AE16" s="3">
+        <f t="shared" si="8"/>
+        <v>3.90625</v>
+      </c>
+      <c r="AF16" s="20">
+        <f t="shared" si="9"/>
+        <v>-6.227106227106232E-2</v>
+      </c>
+      <c r="AG16" s="9"/>
+    </row>
+    <row r="17" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" t="s">
         <v>25</v>
@@ -1695,7 +1857,7 @@
         <v>0.105</v>
       </c>
       <c r="Q17" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.6630036630036629</v>
       </c>
       <c r="R17" s="9"/>
@@ -1724,8 +1886,20 @@
         <v>0.23076923076923075</v>
       </c>
       <c r="AB17" s="9"/>
-    </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD17" s="3">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AE17" s="3">
+        <f t="shared" si="8"/>
+        <v>3.6231884057971011</v>
+      </c>
+      <c r="AF17" s="20">
+        <f t="shared" si="9"/>
+        <v>1.0989010989010999E-2</v>
+      </c>
+      <c r="AG17" s="9"/>
+    </row>
+    <row r="18" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
       <c r="C18" t="s">
         <v>26</v>
@@ -1762,7 +1936,7 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="Q18" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.734129947722181</v>
       </c>
       <c r="R18" s="9"/>
@@ -1791,8 +1965,20 @@
         <v>0.24271844660194178</v>
       </c>
       <c r="AB18" s="9"/>
-    </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD18" s="3">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="AE18" s="3">
+        <f t="shared" si="8"/>
+        <v>3.7313432835820892</v>
+      </c>
+      <c r="AF18" s="20">
+        <f t="shared" si="9"/>
+        <v>7.4682598954456121E-4</v>
+      </c>
+      <c r="AG18" s="9"/>
+    </row>
+    <row r="19" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B19" s="8"/>
       <c r="C19" t="s">
         <v>13</v>
@@ -1829,7 +2015,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="Q19" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.9623233908948192</v>
       </c>
       <c r="R19" s="9"/>
@@ -1858,8 +2044,20 @@
         <v>-2.0408163265306159E-2</v>
       </c>
       <c r="AB19" s="9"/>
-    </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD19" s="19">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AE19" s="3">
+        <f t="shared" si="8"/>
+        <v>1.9083969465648853</v>
+      </c>
+      <c r="AF19" s="20">
+        <f t="shared" si="9"/>
+        <v>2.8257456828885336E-2</v>
+      </c>
+      <c r="AG19" s="9"/>
+    </row>
+    <row r="20" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
       <c r="C20" t="s">
         <v>27</v>
@@ -1896,7 +2094,7 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="Q20" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.9723865877712032</v>
       </c>
       <c r="R20" s="9"/>
@@ -1925,8 +2123,20 @@
         <v>-1.5384615384615332E-2</v>
       </c>
       <c r="AB20" s="9"/>
-    </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD20" s="3">
+        <v>0.126</v>
+      </c>
+      <c r="AE20" s="3">
+        <f t="shared" si="8"/>
+        <v>1.9841269841269842</v>
+      </c>
+      <c r="AF20" s="20">
+        <f t="shared" si="9"/>
+        <v>-5.9171597633136145E-3</v>
+      </c>
+      <c r="AG20" s="9"/>
+    </row>
+    <row r="21" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" t="s">
         <v>28</v>
@@ -1963,7 +2173,7 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="Q21" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.935995302407516</v>
       </c>
       <c r="R21" s="9"/>
@@ -1992,8 +2202,20 @@
         <v>-1.3505578391074554E-2</v>
       </c>
       <c r="AB21" s="9"/>
-    </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD21" s="3">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="AE21" s="3">
+        <f t="shared" si="8"/>
+        <v>3.7878787878787876</v>
+      </c>
+      <c r="AF21" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.22489724016441573</v>
+      </c>
+      <c r="AG21" s="9"/>
+    </row>
+    <row r="22" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="C22" t="s">
         <v>29</v>
@@ -2030,7 +2252,7 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="Q22" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.935995302407516</v>
       </c>
       <c r="R22" s="9"/>
@@ -2059,8 +2281,20 @@
         <v>-1.3505578391074554E-2</v>
       </c>
       <c r="AB22" s="9"/>
-    </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD22" s="3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="AE22" s="3">
+        <f t="shared" si="8"/>
+        <v>3.90625</v>
+      </c>
+      <c r="AF22" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.24838520258367588</v>
+      </c>
+      <c r="AG22" s="9"/>
+    </row>
+    <row r="23" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B23" s="8"/>
       <c r="C23" t="s">
         <v>30</v>
@@ -2097,7 +2331,7 @@
         <v>0.14599999999999999</v>
       </c>
       <c r="Q23" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.6343519494204428</v>
       </c>
       <c r="R23" s="9"/>
@@ -2126,8 +2360,20 @@
         <v>-0.12328767123287673</v>
       </c>
       <c r="AB23" s="9"/>
-    </row>
-    <row r="24" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD23" s="3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="AE23" s="3">
+        <f t="shared" si="8"/>
+        <v>3.90625</v>
+      </c>
+      <c r="AF23" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.32560590094836667</v>
+      </c>
+      <c r="AG23" s="9"/>
+    </row>
+    <row r="24" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B24" s="8"/>
       <c r="C24" t="s">
         <v>14</v>
@@ -2164,7 +2410,7 @@
         <v>0.34</v>
       </c>
       <c r="Q24" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.1312217194570133</v>
       </c>
       <c r="R24" s="9"/>
@@ -2193,8 +2439,20 @@
         <v>-0.43529411764705889</v>
       </c>
       <c r="AB24" s="9"/>
-    </row>
-    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD24" s="19">
+        <v>0.124</v>
+      </c>
+      <c r="AE24" s="3">
+        <f t="shared" si="8"/>
+        <v>2.0161290322580645</v>
+      </c>
+      <c r="AF24" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.43891402714932137</v>
+      </c>
+      <c r="AG24" s="9"/>
+    </row>
+    <row r="25" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B25" s="8"/>
       <c r="C25" t="s">
         <v>31</v>
@@ -2231,7 +2489,7 @@
         <v>0.33900000000000002</v>
       </c>
       <c r="Q25" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.1345586566825503</v>
       </c>
       <c r="R25" s="9"/>
@@ -2260,8 +2518,20 @@
         <v>-0.4336283185840708</v>
       </c>
       <c r="AB25" s="9"/>
-    </row>
-    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD25" s="3">
+        <v>0.124</v>
+      </c>
+      <c r="AE25" s="3">
+        <f t="shared" si="8"/>
+        <v>2.0161290322580645</v>
+      </c>
+      <c r="AF25" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.437258906285455</v>
+      </c>
+      <c r="AG25" s="9"/>
+    </row>
+    <row r="26" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
       <c r="C26" t="s">
         <v>38</v>
@@ -2285,11 +2555,11 @@
         <v>0.44500000000000001</v>
       </c>
       <c r="L26" s="3">
-        <f t="shared" ref="L26:L32" si="9">1/($K$3*K26)</f>
+        <f t="shared" ref="L26:L32" si="11">1/($K$3*K26)</f>
         <v>0.74906367041198507</v>
       </c>
       <c r="M26" s="20">
-        <f t="shared" ref="M26:M32" si="10">(K26*$K$3 - $P26*$P$3)/($P26*$P$3)</f>
+        <f t="shared" ref="M26:M32" si="12">(K26*$K$3 - $P26*$P$3)/($P26*$P$3)</f>
         <v>1.2922390109890107</v>
       </c>
       <c r="N26" s="9"/>
@@ -2298,7 +2568,7 @@
         <v>0.224</v>
       </c>
       <c r="Q26" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.7170329670329669</v>
       </c>
       <c r="R26" s="9"/>
@@ -2319,16 +2589,28 @@
         <v>0.105</v>
       </c>
       <c r="Z26" s="3">
-        <f t="shared" ref="Z26:Z36" si="11">1/($Y$3*Y26)</f>
+        <f t="shared" ref="Z26:Z36" si="13">1/($Y$3*Y26)</f>
         <v>2.9761904761904758</v>
       </c>
       <c r="AA26" s="20">
-        <f t="shared" ref="AA26:AA36" si="12">(Y26*$Y$3 - $P26*$P$3)/($P26*$P$3)</f>
+        <f t="shared" ref="AA26:AA36" si="14">(Y26*$Y$3 - $P26*$P$3)/($P26*$P$3)</f>
         <v>-0.42307692307692307</v>
       </c>
       <c r="AB26" s="9"/>
-    </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD26" s="3">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AE26" s="3">
+        <f t="shared" si="8"/>
+        <v>3.0487804878048781</v>
+      </c>
+      <c r="AF26" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.43681318681318682</v>
+      </c>
+      <c r="AG26" s="9"/>
+    </row>
+    <row r="27" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
       <c r="C27" t="s">
         <v>39</v>
@@ -2352,11 +2634,11 @@
         <v>0.44500000000000001</v>
       </c>
       <c r="L27" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.74906367041198507</v>
       </c>
       <c r="M27" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>1.4450549450549448</v>
       </c>
       <c r="N27" s="9"/>
@@ -2365,7 +2647,7 @@
         <v>0.21</v>
       </c>
       <c r="Q27" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.8315018315018314</v>
       </c>
       <c r="R27" s="9"/>
@@ -2386,16 +2668,28 @@
         <v>0.105</v>
       </c>
       <c r="Z27" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.9761904761904758</v>
       </c>
       <c r="AA27" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.38461538461538464</v>
       </c>
       <c r="AB27" s="9"/>
-    </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD27" s="3">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AE27" s="3">
+        <f t="shared" si="8"/>
+        <v>3.0487804878048781</v>
+      </c>
+      <c r="AF27" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.39926739926739929</v>
+      </c>
+      <c r="AG27" s="9"/>
+    </row>
+    <row r="28" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
       <c r="C28" t="s">
         <v>40</v>
@@ -2419,11 +2713,11 @@
         <v>0.44500000000000001</v>
       </c>
       <c r="L28" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.74906367041198507</v>
       </c>
       <c r="M28" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>2.5657051282051277</v>
       </c>
       <c r="N28" s="9"/>
@@ -2432,7 +2726,7 @@
         <v>0.14399999999999999</v>
       </c>
       <c r="Q28" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2.6709401709401708</v>
       </c>
       <c r="R28" s="9"/>
@@ -2453,16 +2747,28 @@
         <v>0.11700000000000001</v>
       </c>
       <c r="Z28" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.6709401709401703</v>
       </c>
       <c r="AA28" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>1.4826696375870145E-16</v>
       </c>
       <c r="AB28" s="9"/>
-    </row>
-    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD28" s="3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="AE28" s="3">
+        <f t="shared" si="8"/>
+        <v>5.3191489361702127</v>
+      </c>
+      <c r="AF28" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.49786324786324787</v>
+      </c>
+      <c r="AG28" s="9"/>
+    </row>
+    <row r="29" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B29" s="8"/>
       <c r="C29" t="s">
         <v>41</v>
@@ -2486,11 +2792,11 @@
         <v>0.44500000000000001</v>
       </c>
       <c r="L29" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.74906367041198507</v>
       </c>
       <c r="M29" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.4223311314724057</v>
       </c>
       <c r="N29" s="9"/>
@@ -2499,7 +2805,7 @@
         <v>0.36099999999999999</v>
       </c>
       <c r="Q29" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.0654165778819518</v>
       </c>
       <c r="R29" s="9"/>
@@ -2520,16 +2826,28 @@
         <v>0.21</v>
       </c>
       <c r="Z29" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.4880952380952379</v>
       </c>
       <c r="AA29" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.28404005966332829</v>
       </c>
       <c r="AB29" s="9"/>
-    </row>
-    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD29" s="3">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AE29" s="3">
+        <f t="shared" si="8"/>
+        <v>1.4880952380952379</v>
+      </c>
+      <c r="AF29" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.28404005966332829</v>
+      </c>
+      <c r="AG29" s="9"/>
+    </row>
+    <row r="30" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
       <c r="C30" t="s">
         <v>42</v>
@@ -2553,11 +2871,11 @@
         <v>0.44500000000000001</v>
       </c>
       <c r="L30" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.74906367041198507</v>
       </c>
       <c r="M30" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>3.5439074200136145</v>
       </c>
       <c r="N30" s="9"/>
@@ -2566,7 +2884,7 @@
         <v>0.113</v>
       </c>
       <c r="Q30" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.4036759700476513</v>
       </c>
       <c r="R30" s="9"/>
@@ -2587,16 +2905,28 @@
         <v>9.8000000000000004E-2</v>
       </c>
       <c r="Z30" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.1887755102040813</v>
       </c>
       <c r="AA30" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6.739278420694364E-2</v>
       </c>
       <c r="AB30" s="9"/>
-    </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD30" s="3">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="AE30" s="3">
+        <f t="shared" si="8"/>
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="AF30" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.38733832539142277</v>
+      </c>
+      <c r="AG30" s="9"/>
+    </row>
+    <row r="31" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
       <c r="C31" t="s">
         <v>43</v>
@@ -2620,11 +2950,11 @@
         <v>0.44500000000000001</v>
       </c>
       <c r="L31" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.74906367041198507</v>
       </c>
       <c r="M31" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.52362474320931274</v>
       </c>
       <c r="N31" s="9"/>
@@ -2633,7 +2963,7 @@
         <v>0.33700000000000002</v>
       </c>
       <c r="Q31" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1.1412919424788859</v>
       </c>
       <c r="R31" s="9"/>
@@ -2654,16 +2984,28 @@
         <v>0.21</v>
       </c>
       <c r="Z31" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>1.4880952380952379</v>
       </c>
       <c r="AA31" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>-0.23305181465418856</v>
       </c>
       <c r="AB31" s="9"/>
-    </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD31" s="3">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="AE31" s="3">
+        <f t="shared" si="8"/>
+        <v>1.4450867052023122</v>
+      </c>
+      <c r="AF31" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.21022597580461097</v>
+      </c>
+      <c r="AG31" s="9"/>
+    </row>
+    <row r="32" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
       <c r="C32" t="s">
         <v>15</v>
@@ -2687,11 +3029,11 @@
         <v>0.58399999999999996</v>
       </c>
       <c r="L32" s="3">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.57077625570776258</v>
       </c>
       <c r="M32" s="20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4.4784240150093799</v>
       </c>
       <c r="N32" s="9"/>
@@ -2700,7 +3042,7 @@
         <v>0.123</v>
       </c>
       <c r="Q32" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>3.1269543464665412</v>
       </c>
       <c r="R32" s="9"/>
@@ -2721,16 +3063,28 @@
         <v>0.104</v>
       </c>
       <c r="Z32" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>3.0048076923076925</v>
       </c>
       <c r="AA32" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>4.0650406504064901E-2</v>
       </c>
       <c r="AB32" s="9"/>
-    </row>
-    <row r="33" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD32" s="3">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="AE32" s="3">
+        <f t="shared" si="8"/>
+        <v>3.7313432835820892</v>
+      </c>
+      <c r="AF32" s="20">
+        <f t="shared" si="9"/>
+        <v>-0.16197623514696688</v>
+      </c>
+      <c r="AG32" s="9"/>
+    </row>
+    <row r="33" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B33" s="8"/>
       <c r="C33" t="s">
         <v>16</v>
@@ -2751,7 +3105,7 @@
         <v>0.38500000000000001</v>
       </c>
       <c r="Q33" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99900099900099892</v>
       </c>
       <c r="R33" s="9"/>
@@ -2764,16 +3118,20 @@
         <v>0.313</v>
       </c>
       <c r="Z33" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99840255591054305</v>
       </c>
       <c r="AA33" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>5.9940059940053337E-4</v>
       </c>
       <c r="AB33" s="9"/>
-    </row>
-    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="20"/>
+      <c r="AG33" s="9"/>
+    </row>
+    <row r="34" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B34" s="8"/>
       <c r="C34" t="s">
         <v>17</v>
@@ -2790,7 +3148,7 @@
         <v>0.38500000000000001</v>
       </c>
       <c r="Q34" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99900099900099892</v>
       </c>
       <c r="R34" s="9"/>
@@ -2801,16 +3159,20 @@
         <v>0.313</v>
       </c>
       <c r="Z34" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99840255591054305</v>
       </c>
       <c r="AA34" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>5.9940059940053337E-4</v>
       </c>
       <c r="AB34" s="9"/>
-    </row>
-    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="20"/>
+      <c r="AG34" s="9"/>
+    </row>
+    <row r="35" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B35" s="8"/>
       <c r="C35" t="s">
         <v>32</v>
@@ -2827,7 +3189,7 @@
         <v>0.38500000000000001</v>
       </c>
       <c r="Q35" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99900099900099892</v>
       </c>
       <c r="R35" s="9"/>
@@ -2838,16 +3200,20 @@
         <v>0.313</v>
       </c>
       <c r="Z35" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99840255591054305</v>
       </c>
       <c r="AA35" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>5.9940059940053337E-4</v>
       </c>
       <c r="AB35" s="9"/>
-    </row>
-    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD35" s="3"/>
+      <c r="AE35" s="3"/>
+      <c r="AF35" s="20"/>
+      <c r="AG35" s="9"/>
+    </row>
+    <row r="36" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B36" s="8"/>
       <c r="C36" t="s">
         <v>18</v>
@@ -2864,7 +3230,7 @@
         <v>0.38500000000000001</v>
       </c>
       <c r="Q36" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.99900099900099892</v>
       </c>
       <c r="R36" s="9"/>
@@ -2875,16 +3241,20 @@
         <v>0.314</v>
       </c>
       <c r="Z36" s="3">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.99522292993630557</v>
       </c>
       <c r="AA36" s="20">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>3.7962037962038214E-3</v>
       </c>
       <c r="AB36" s="9"/>
-    </row>
-    <row r="37" spans="2:28" ht="3.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="20"/>
+      <c r="AG36" s="9"/>
+    </row>
+    <row r="37" spans="2:33" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="10"/>
       <c r="C37" s="11"/>
       <c r="D37" s="13"/>
@@ -2912,8 +3282,13 @@
       <c r="Z37" s="12"/>
       <c r="AA37" s="12"/>
       <c r="AB37" s="13"/>
-    </row>
-    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AC37" s="12"/>
+      <c r="AD37" s="12"/>
+      <c r="AE37" s="12"/>
+      <c r="AF37" s="12"/>
+      <c r="AG37" s="13"/>
+    </row>
+    <row r="39" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
         <v>33</v>
       </c>
@@ -2937,8 +3312,12 @@
         <f>(Y12-Y11)/Y11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD39" s="21">
+        <f>(AD12-AD11)/AD11</f>
+        <v>-2.3255813953488393E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C40" s="1" t="s">
         <v>34</v>
       </c>
@@ -2962,14 +3341,20 @@
         <f>(Y24-Y19)/Y19</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD40" s="21">
+        <f>(AD24-AD19)/AD19</f>
+        <v>-5.3435114503816841E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C42" s="1" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="AD2:AF2"/>
+    <mergeCell ref="AD3:AF3"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="P2:Q2"/>
@@ -2982,7 +3367,7 @@
     <mergeCell ref="T3:V3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="78" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="68" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;A</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
Added PAC on M3
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thierry/Devel/arm-instruction-time/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6406F677-0B02-1841-A6BB-163769D744F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5912B1FF-8964-A943-BA87-00750432447E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11040" yWindow="3040" windowWidth="29000" windowHeight="18740" xr2:uid="{D46DF09C-373D-4B8F-933A-76CBCC1CC5EF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>Apple M1</t>
   </si>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>PACIA</t>
-  </si>
-  <si>
-    <t>AUTIA</t>
   </si>
   <si>
     <t>PACIA ... AUTIA ...</t>
@@ -747,10 +744,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AG42"/>
+  <dimension ref="B1:AG41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD4" sqref="AD4"/>
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -776,7 +773,7 @@
     <row r="2" spans="2:33" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="4"/>
       <c r="C2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="4"/>
@@ -801,7 +798,7 @@
       <c r="R2" s="7"/>
       <c r="S2" s="4"/>
       <c r="T2" s="22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="U2" s="22"/>
       <c r="V2" s="22"/>
@@ -815,7 +812,7 @@
       <c r="AB2" s="7"/>
       <c r="AC2" s="6"/>
       <c r="AD2" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AE2" s="22"/>
       <c r="AF2" s="22"/>
@@ -824,7 +821,7 @@
     <row r="3" spans="2:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B3" s="8"/>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="8"/>
@@ -870,70 +867,70 @@
     <row r="4" spans="2:33" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="14"/>
       <c r="C4" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="14"/>
       <c r="F4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G4" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="14"/>
       <c r="K4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M4" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N4" s="16"/>
       <c r="O4" s="14"/>
       <c r="P4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R4" s="16"/>
       <c r="S4" s="14"/>
       <c r="T4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="U4" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="V4" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="W4" s="16"/>
       <c r="X4" s="18"/>
       <c r="Y4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Z4" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AA4" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AB4" s="16"/>
       <c r="AC4" s="18"/>
       <c r="AD4" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AE4" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="AF4" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AG4" s="16"/>
     </row>
@@ -1018,15 +1015,15 @@
       </c>
       <c r="AB6" s="9"/>
       <c r="AD6" s="3">
-        <v>3.2000000000000001E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="AE6" s="3">
         <f>1/($AD$3*AD6)</f>
-        <v>7.8125</v>
+        <v>7.5757575757575752</v>
       </c>
       <c r="AF6" s="20">
         <f>(AD6*$AD$3 - $P6*$P$3)/($P6*$P$3)</f>
-        <v>0.36752136752136749</v>
+        <v>0.4102564102564103</v>
       </c>
       <c r="AG6" s="9"/>
     </row>
@@ -1097,15 +1094,15 @@
       </c>
       <c r="AB7" s="9"/>
       <c r="AD7" s="3">
-        <v>3.7999999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="AE7" s="3">
         <f t="shared" ref="AE7:AE32" si="8">1/($AD$3*AD7)</f>
-        <v>6.5789473684210531</v>
+        <v>6.9444444444444446</v>
       </c>
       <c r="AF7" s="20">
         <f t="shared" ref="AF7:AF32" si="9">(AD7*$AD$3 - $P7*$P$3)/($P7*$P$3)</f>
-        <v>-0.40947940947940953</v>
+        <v>-0.44055944055944063</v>
       </c>
       <c r="AG7" s="9"/>
     </row>
@@ -1146,7 +1143,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="Q8" s="3">
-        <f t="shared" ref="Q8:Q36" si="10">1/($P$3*P8)</f>
+        <f t="shared" ref="Q8:Q35" si="10">1/($P$3*P8)</f>
         <v>3.8850038850038846</v>
       </c>
       <c r="R8" s="9"/>
@@ -1176,15 +1173,15 @@
       </c>
       <c r="AB8" s="9"/>
       <c r="AD8" s="3">
-        <v>6.8000000000000005E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="AE8" s="3">
         <f t="shared" si="8"/>
-        <v>3.6764705882352939</v>
+        <v>3.8461538461538458</v>
       </c>
       <c r="AF8" s="20">
         <f t="shared" si="9"/>
-        <v>5.6721056721056727E-2</v>
+        <v>1.0101010101010065E-2</v>
       </c>
       <c r="AG8" s="9"/>
     </row>
@@ -1255,15 +1252,15 @@
       </c>
       <c r="AB9" s="9"/>
       <c r="AD9" s="3">
-        <v>7.0000000000000007E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="AE9" s="3">
         <f t="shared" si="8"/>
-        <v>3.5714285714285712</v>
+        <v>3.7878787878787876</v>
       </c>
       <c r="AF9" s="20">
         <f t="shared" si="9"/>
-        <v>-0.17792131532589545</v>
+        <v>-0.22489724016441573</v>
       </c>
       <c r="AG9" s="9"/>
     </row>
@@ -1334,15 +1331,15 @@
       </c>
       <c r="AB10" s="9"/>
       <c r="AD10" s="3">
-        <v>0.253</v>
+        <v>0.249</v>
       </c>
       <c r="AE10" s="3">
         <f t="shared" si="8"/>
-        <v>0.98814229249011853</v>
+        <v>1.0040160642570282</v>
       </c>
       <c r="AF10" s="20">
         <f t="shared" si="9"/>
-        <v>3.1720856463123208E-3</v>
+        <v>-1.2688342585249944E-2</v>
       </c>
       <c r="AG10" s="9"/>
     </row>
@@ -1413,15 +1410,15 @@
       </c>
       <c r="AB11" s="9"/>
       <c r="AD11" s="19">
-        <v>0.129</v>
+        <v>0.126</v>
       </c>
       <c r="AE11" s="3">
         <f t="shared" si="8"/>
-        <v>1.9379844961240309</v>
+        <v>1.9841269841269842</v>
       </c>
       <c r="AF11" s="20">
         <f t="shared" si="9"/>
-        <v>2.829812674372258E-2</v>
+        <v>4.3842168194499391E-3</v>
       </c>
       <c r="AG11" s="9"/>
     </row>
@@ -1507,7 +1504,7 @@
     <row r="13" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B13" s="8"/>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="8"/>
@@ -1571,15 +1568,15 @@
       </c>
       <c r="AB13" s="9"/>
       <c r="AD13" s="3">
-        <v>0.496</v>
+        <v>0.498</v>
       </c>
       <c r="AE13" s="3">
         <f t="shared" si="8"/>
-        <v>0.50403225806451613</v>
+        <v>0.50200803212851408</v>
       </c>
       <c r="AF13" s="20">
         <f t="shared" si="9"/>
-        <v>-0.6698066105249143</v>
+        <v>-0.66847518556735352</v>
       </c>
       <c r="AG13" s="9"/>
     </row>
@@ -1650,15 +1647,15 @@
       </c>
       <c r="AB14" s="9"/>
       <c r="AD14" s="3">
-        <v>0.124</v>
+        <v>0.125</v>
       </c>
       <c r="AE14" s="3">
         <f t="shared" si="8"/>
-        <v>2.0161290322580645</v>
+        <v>2</v>
       </c>
       <c r="AF14" s="20">
         <f t="shared" si="9"/>
-        <v>-1.155838979673182E-2</v>
+        <v>-3.58708648864094E-3</v>
       </c>
       <c r="AG14" s="9"/>
     </row>
@@ -1729,22 +1726,22 @@
       </c>
       <c r="AB15" s="9"/>
       <c r="AD15" s="3">
-        <v>0.124</v>
+        <v>0.125</v>
       </c>
       <c r="AE15" s="3">
         <f t="shared" si="8"/>
-        <v>2.0161290322580645</v>
+        <v>2</v>
       </c>
       <c r="AF15" s="20">
         <f t="shared" si="9"/>
-        <v>-0.3511250654107797</v>
+        <v>-0.34589220303506013</v>
       </c>
       <c r="AG15" s="9"/>
     </row>
     <row r="16" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B16" s="8"/>
       <c r="C16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
@@ -1808,22 +1805,22 @@
       </c>
       <c r="AB16" s="9"/>
       <c r="AD16" s="3">
-        <v>6.4000000000000001E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="AE16" s="3">
         <f t="shared" si="8"/>
-        <v>3.90625</v>
+        <v>3.9682539682539684</v>
       </c>
       <c r="AF16" s="20">
         <f t="shared" si="9"/>
-        <v>-6.227106227106232E-2</v>
+        <v>-7.6923076923076983E-2</v>
       </c>
       <c r="AG16" s="9"/>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="8"/>
@@ -1887,22 +1884,22 @@
       </c>
       <c r="AB17" s="9"/>
       <c r="AD17" s="3">
-        <v>6.9000000000000006E-2</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="AE17" s="3">
         <f t="shared" si="8"/>
-        <v>3.6231884057971011</v>
+        <v>3.90625</v>
       </c>
       <c r="AF17" s="20">
         <f t="shared" si="9"/>
-        <v>1.0989010989010999E-2</v>
+        <v>-6.227106227106232E-2</v>
       </c>
       <c r="AG17" s="9"/>
     </row>
     <row r="18" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
       <c r="C18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="8"/>
@@ -1966,15 +1963,15 @@
       </c>
       <c r="AB18" s="9"/>
       <c r="AD18" s="3">
-        <v>6.7000000000000004E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="AE18" s="3">
         <f t="shared" si="8"/>
-        <v>3.7313432835820892</v>
+        <v>3.9682539682539684</v>
       </c>
       <c r="AF18" s="20">
         <f t="shared" si="9"/>
-        <v>7.4682598954456121E-4</v>
+        <v>-5.8999253174010384E-2</v>
       </c>
       <c r="AG18" s="9"/>
     </row>
@@ -2045,22 +2042,22 @@
       </c>
       <c r="AB19" s="9"/>
       <c r="AD19" s="19">
-        <v>0.13100000000000001</v>
+        <v>0.124</v>
       </c>
       <c r="AE19" s="3">
         <f t="shared" si="8"/>
-        <v>1.9083969465648853</v>
+        <v>2.0161290322580645</v>
       </c>
       <c r="AF19" s="20">
         <f t="shared" si="9"/>
-        <v>2.8257456828885336E-2</v>
+        <v>-2.6687598116169654E-2</v>
       </c>
       <c r="AG19" s="9"/>
     </row>
     <row r="20" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="8"/>
@@ -2124,22 +2121,22 @@
       </c>
       <c r="AB20" s="9"/>
       <c r="AD20" s="3">
-        <v>0.126</v>
+        <v>0.125</v>
       </c>
       <c r="AE20" s="3">
         <f t="shared" si="8"/>
-        <v>1.9841269841269842</v>
+        <v>2</v>
       </c>
       <c r="AF20" s="20">
         <f t="shared" si="9"/>
-        <v>-5.9171597633136145E-3</v>
+        <v>-1.3806706114398434E-2</v>
       </c>
       <c r="AG20" s="9"/>
     </row>
     <row r="21" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
@@ -2203,22 +2200,22 @@
       </c>
       <c r="AB21" s="9"/>
       <c r="AD21" s="3">
-        <v>6.6000000000000003E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="AE21" s="3">
         <f t="shared" si="8"/>
-        <v>3.7878787878787876</v>
+        <v>4.032258064516129</v>
       </c>
       <c r="AF21" s="20">
         <f t="shared" si="9"/>
-        <v>-0.22489724016441573</v>
+        <v>-0.27187316500293601</v>
       </c>
       <c r="AG21" s="9"/>
     </row>
     <row r="22" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="C22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="8"/>
@@ -2282,22 +2279,22 @@
       </c>
       <c r="AB22" s="9"/>
       <c r="AD22" s="3">
-        <v>6.4000000000000001E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="AE22" s="3">
         <f t="shared" si="8"/>
-        <v>3.90625</v>
+        <v>4.032258064516129</v>
       </c>
       <c r="AF22" s="20">
         <f t="shared" si="9"/>
-        <v>-0.24838520258367588</v>
+        <v>-0.27187316500293601</v>
       </c>
       <c r="AG22" s="9"/>
     </row>
     <row r="23" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B23" s="8"/>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="8"/>
@@ -2361,15 +2358,15 @@
       </c>
       <c r="AB23" s="9"/>
       <c r="AD23" s="3">
-        <v>6.4000000000000001E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="AE23" s="3">
         <f t="shared" si="8"/>
-        <v>3.90625</v>
+        <v>3.9682539682539684</v>
       </c>
       <c r="AF23" s="20">
         <f t="shared" si="9"/>
-        <v>-0.32560590094836667</v>
+        <v>-0.33614330874604847</v>
       </c>
       <c r="AG23" s="9"/>
     </row>
@@ -2455,7 +2452,7 @@
     <row r="25" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B25" s="8"/>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="8"/>
@@ -2519,22 +2516,22 @@
       </c>
       <c r="AB25" s="9"/>
       <c r="AD25" s="3">
-        <v>0.124</v>
+        <v>0.125</v>
       </c>
       <c r="AE25" s="3">
         <f t="shared" si="8"/>
-        <v>2.0161290322580645</v>
+        <v>2</v>
       </c>
       <c r="AF25" s="20">
         <f t="shared" si="9"/>
-        <v>-0.437258906285455</v>
+        <v>-0.4327206716587248</v>
       </c>
       <c r="AG25" s="9"/>
     </row>
     <row r="26" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B26" s="8"/>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="8"/>
@@ -2589,31 +2586,31 @@
         <v>0.105</v>
       </c>
       <c r="Z26" s="3">
-        <f t="shared" ref="Z26:Z36" si="13">1/($Y$3*Y26)</f>
+        <f t="shared" ref="Z26:Z35" si="13">1/($Y$3*Y26)</f>
         <v>2.9761904761904758</v>
       </c>
       <c r="AA26" s="20">
-        <f t="shared" ref="AA26:AA36" si="14">(Y26*$Y$3 - $P26*$P$3)/($P26*$P$3)</f>
+        <f t="shared" ref="AA26:AA35" si="14">(Y26*$Y$3 - $P26*$P$3)/($P26*$P$3)</f>
         <v>-0.42307692307692307</v>
       </c>
       <c r="AB26" s="9"/>
       <c r="AD26" s="3">
-        <v>8.2000000000000003E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="AE26" s="3">
         <f t="shared" si="8"/>
-        <v>3.0487804878048781</v>
+        <v>3.012048192771084</v>
       </c>
       <c r="AF26" s="20">
         <f t="shared" si="9"/>
-        <v>-0.43681318681318682</v>
+        <v>-0.42994505494505492</v>
       </c>
       <c r="AG26" s="9"/>
     </row>
     <row r="27" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
       <c r="C27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
@@ -2677,22 +2674,22 @@
       </c>
       <c r="AB27" s="9"/>
       <c r="AD27" s="3">
-        <v>8.2000000000000003E-2</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="AE27" s="3">
         <f t="shared" si="8"/>
-        <v>3.0487804878048781</v>
+        <v>3.012048192771084</v>
       </c>
       <c r="AF27" s="20">
         <f t="shared" si="9"/>
-        <v>-0.39926739926739929</v>
+        <v>-0.39194139194139194</v>
       </c>
       <c r="AG27" s="9"/>
     </row>
     <row r="28" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
@@ -2756,22 +2753,22 @@
       </c>
       <c r="AB28" s="9"/>
       <c r="AD28" s="3">
-        <v>4.7E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="AE28" s="3">
         <f t="shared" si="8"/>
-        <v>5.3191489361702127</v>
+        <v>5.4347826086956523</v>
       </c>
       <c r="AF28" s="20">
         <f t="shared" si="9"/>
-        <v>-0.49786324786324787</v>
+        <v>-0.50854700854700852</v>
       </c>
       <c r="AG28" s="9"/>
     </row>
     <row r="29" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B29" s="8"/>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
@@ -2835,22 +2832,22 @@
       </c>
       <c r="AB29" s="9"/>
       <c r="AD29" s="3">
-        <v>0.16800000000000001</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="AE29" s="3">
         <f t="shared" si="8"/>
-        <v>1.4880952380952379</v>
+        <v>1.506024096385542</v>
       </c>
       <c r="AF29" s="20">
         <f t="shared" si="9"/>
-        <v>-0.28404005966332829</v>
+        <v>-0.29256339228638395</v>
       </c>
       <c r="AG29" s="9"/>
     </row>
     <row r="30" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="8"/>
@@ -2929,7 +2926,7 @@
     <row r="31" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="9"/>
       <c r="E31" s="8"/>
@@ -2993,15 +2990,15 @@
       </c>
       <c r="AB31" s="9"/>
       <c r="AD31" s="3">
-        <v>0.17299999999999999</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="AE31" s="3">
         <f t="shared" si="8"/>
-        <v>1.4450867052023122</v>
+        <v>1.4970059880239519</v>
       </c>
       <c r="AF31" s="20">
         <f t="shared" si="9"/>
-        <v>-0.21022597580461097</v>
+        <v>-0.23761698242410412</v>
       </c>
       <c r="AG31" s="9"/>
     </row>
@@ -3072,15 +3069,15 @@
       </c>
       <c r="AB32" s="9"/>
       <c r="AD32" s="3">
-        <v>6.7000000000000004E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="AE32" s="3">
         <f t="shared" si="8"/>
-        <v>3.7313432835820892</v>
+        <v>3.9682539682539684</v>
       </c>
       <c r="AF32" s="20">
         <f t="shared" si="9"/>
-        <v>-0.16197623514696688</v>
+        <v>-0.21200750469043159</v>
       </c>
       <c r="AG32" s="9"/>
     </row>
@@ -3126,15 +3123,23 @@
         <v>5.9940059940053337E-4</v>
       </c>
       <c r="AB33" s="9"/>
-      <c r="AD33" s="3"/>
-      <c r="AE33" s="3"/>
-      <c r="AF33" s="20"/>
+      <c r="AD33" s="3">
+        <v>0.248</v>
+      </c>
+      <c r="AE33" s="3">
+        <f t="shared" ref="AE33:AE35" si="15">1/($AD$3*AD33)</f>
+        <v>1.0080645161290323</v>
+      </c>
+      <c r="AF33" s="20">
+        <f t="shared" ref="AF33:AF35" si="16">(AD33*$AD$3 - $P33*$P$3)/($P33*$P$3)</f>
+        <v>-8.9910089910091081E-3</v>
+      </c>
       <c r="AG33" s="9"/>
     </row>
     <row r="34" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B34" s="8"/>
       <c r="C34" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
@@ -3167,15 +3172,23 @@
         <v>5.9940059940053337E-4</v>
       </c>
       <c r="AB34" s="9"/>
-      <c r="AD34" s="3"/>
-      <c r="AE34" s="3"/>
-      <c r="AF34" s="20"/>
+      <c r="AD34" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="AE34" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+      <c r="AF34" s="20">
+        <f t="shared" si="16"/>
+        <v>-9.9900099900111067E-4</v>
+      </c>
       <c r="AG34" s="9"/>
     </row>
     <row r="35" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B35" s="8"/>
       <c r="C35" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
@@ -3197,174 +3210,141 @@
       <c r="T35" s="3"/>
       <c r="W35" s="9"/>
       <c r="Y35" s="3">
-        <v>0.313</v>
+        <v>0.314</v>
       </c>
       <c r="Z35" s="3">
         <f t="shared" si="13"/>
-        <v>0.99840255591054305</v>
+        <v>0.99522292993630557</v>
       </c>
       <c r="AA35" s="20">
         <f t="shared" si="14"/>
-        <v>5.9940059940053337E-4</v>
+        <v>3.7962037962038214E-3</v>
       </c>
       <c r="AB35" s="9"/>
-      <c r="AD35" s="3"/>
-      <c r="AE35" s="3"/>
-      <c r="AF35" s="20"/>
+      <c r="AD35" s="3">
+        <v>0.251</v>
+      </c>
+      <c r="AE35" s="3">
+        <f t="shared" si="15"/>
+        <v>0.99601593625498008</v>
+      </c>
+      <c r="AF35" s="20">
+        <f t="shared" si="16"/>
+        <v>2.9970029970028886E-3</v>
+      </c>
       <c r="AG35" s="9"/>
     </row>
-    <row r="36" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B36" s="8"/>
-      <c r="C36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="3"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="3"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="3">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="Q36" s="3">
-        <f t="shared" si="10"/>
-        <v>0.99900099900099892</v>
-      </c>
-      <c r="R36" s="9"/>
-      <c r="S36" s="8"/>
-      <c r="T36" s="3"/>
-      <c r="W36" s="9"/>
-      <c r="Y36" s="3">
-        <v>0.314</v>
-      </c>
-      <c r="Z36" s="3">
-        <f t="shared" si="13"/>
-        <v>0.99522292993630557</v>
-      </c>
-      <c r="AA36" s="20">
-        <f t="shared" si="14"/>
-        <v>3.7962037962038214E-3</v>
-      </c>
-      <c r="AB36" s="9"/>
-      <c r="AD36" s="3"/>
-      <c r="AE36" s="3"/>
-      <c r="AF36" s="20"/>
-      <c r="AG36" s="9"/>
-    </row>
-    <row r="37" spans="2:33" ht="4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="10"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="10"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="13"/>
-      <c r="O37" s="10"/>
-      <c r="P37" s="12"/>
-      <c r="Q37" s="12"/>
-      <c r="R37" s="13"/>
-      <c r="S37" s="10"/>
-      <c r="T37" s="12"/>
-      <c r="U37" s="12"/>
-      <c r="V37" s="12"/>
-      <c r="W37" s="13"/>
-      <c r="X37" s="12"/>
-      <c r="Y37" s="12"/>
-      <c r="Z37" s="12"/>
-      <c r="AA37" s="12"/>
-      <c r="AB37" s="13"/>
-      <c r="AC37" s="12"/>
-      <c r="AD37" s="12"/>
-      <c r="AE37" s="12"/>
-      <c r="AF37" s="12"/>
-      <c r="AG37" s="13"/>
+    <row r="36" spans="2:33" ht="4" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="10"/>
+      <c r="C36" s="11"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="10"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="10"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="12"/>
+      <c r="W36" s="13"/>
+      <c r="X36" s="12"/>
+      <c r="Y36" s="12"/>
+      <c r="Z36" s="12"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="13"/>
+      <c r="AC36" s="12"/>
+      <c r="AD36" s="12"/>
+      <c r="AE36" s="12"/>
+      <c r="AF36" s="12"/>
+      <c r="AG36" s="13"/>
+    </row>
+    <row r="38" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="C38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F38" s="21">
+        <f>(F12-F11)/F11</f>
+        <v>0.33333333333333343</v>
+      </c>
+      <c r="K38" s="21">
+        <f>(K12-K11)/K11</f>
+        <v>0.33333333333333343</v>
+      </c>
+      <c r="P38" s="21">
+        <f>(P12-P11)/P11</f>
+        <v>0</v>
+      </c>
+      <c r="T38" s="21">
+        <f>(T12-T11)/T11</f>
+        <v>0</v>
+      </c>
+      <c r="Y38" s="21">
+        <f>(Y12-Y11)/Y11</f>
+        <v>0</v>
+      </c>
+      <c r="AD38" s="21">
+        <f>(AD12-AD11)/AD11</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="2:33" x14ac:dyDescent="0.2">
       <c r="C39" s="1" t="s">
         <v>33</v>
       </c>
       <c r="F39" s="21">
-        <f>(F12-F11)/F11</f>
-        <v>0.33333333333333343</v>
-      </c>
-      <c r="K39" s="21">
-        <f>(K12-K11)/K11</f>
-        <v>0.33333333333333343</v>
-      </c>
-      <c r="P39" s="21">
-        <f>(P12-P11)/P11</f>
-        <v>0</v>
-      </c>
-      <c r="T39" s="21">
-        <f>(T12-T11)/T11</f>
-        <v>0</v>
-      </c>
-      <c r="Y39" s="21">
-        <f>(Y12-Y11)/Y11</f>
-        <v>0</v>
-      </c>
-      <c r="AD39" s="21">
-        <f>(AD12-AD11)/AD11</f>
-        <v>-2.3255813953488393E-2</v>
-      </c>
-    </row>
-    <row r="40" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="C40" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" s="21">
         <f>(F24-F19)/F19</f>
         <v>0.33253873659118016</v>
       </c>
-      <c r="K40" s="21">
+      <c r="K39" s="21">
         <f>(K24-K19)/K19</f>
         <v>0.33333333333333343</v>
       </c>
-      <c r="P40" s="21">
+      <c r="P39" s="21">
         <f>(P24-P19)/P19</f>
         <v>0.73469387755102045</v>
       </c>
-      <c r="T40" s="21">
+      <c r="T39" s="21">
         <f>(T24-T19)/T19</f>
         <v>0.43617021276595752</v>
       </c>
-      <c r="Y40" s="21">
+      <c r="Y39" s="21">
         <f>(Y24-Y19)/Y19</f>
         <v>0</v>
       </c>
-      <c r="AD40" s="21">
+      <c r="AD39" s="21">
         <f>(AD24-AD19)/AD19</f>
-        <v>-5.3435114503816841E-2</v>
-      </c>
-    </row>
-    <row r="42" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="C42" s="1" t="s">
-        <v>37</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="C41" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="T2:V2"/>
+    <mergeCell ref="T3:V3"/>
     <mergeCell ref="AD2:AF2"/>
     <mergeCell ref="AD3:AF3"/>
     <mergeCell ref="Y2:AA2"/>
     <mergeCell ref="Y3:AA3"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="T2:V2"/>
-    <mergeCell ref="T3:V3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="68" orientation="landscape" r:id="rId1"/>

</xml_diff>